<commit_message>
post semi finals update
</commit_message>
<xml_diff>
--- a/ESCAPE Ratings/Spreads/y2024/spreads_tracker_week17.xlsx
+++ b/ESCAPE Ratings/Spreads/y2024/spreads_tracker_week17.xlsx
@@ -713,41 +713,41 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Navy</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>SMU</t>
+          <t>Oklahoma</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>9.5</v>
+        <v>9.4</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Penn State -nan</t>
+          <t>Navy -nan</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Penn State -9</t>
+          <t>Navy -1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Penn State -18.5</t>
+          <t>Oklahoma -8.4</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Penn State -28.0</t>
+          <t>Navy -1.0</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -757,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -766,41 +766,41 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Navy</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Oklahoma</t>
+          <t>SMU</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9.4</v>
+        <v>8.5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Navy -nan</t>
+          <t>Penn State -nan</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Navy -1</t>
+          <t>Penn State -9</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Oklahoma -8.4</t>
+          <t>Penn State -17.5</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I7" t="n">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Navy -1.0</t>
+          <t>Penn State -28.0</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -810,7 +810,7 @@
         <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -828,7 +828,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8.300000000000001</v>
+        <v>8</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -842,7 +842,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>South Alabama -14.3</t>
+          <t>South Alabama -14.0</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -925,12 +925,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Texas Tech</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -938,39 +938,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Arkansas -2.5</t>
+          <t>Notre Dame -nan</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Texas Tech -3.5</t>
+          <t>Ohio State -9.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Arkansas -4.4</t>
+          <t>Ohio State -1.6</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>-3.5</v>
-      </c>
-      <c r="I10" t="n">
-        <v>13</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Arkansas -13.0</t>
-        </is>
-      </c>
-      <c r="K10" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" t="n">
-        <v>1</v>
-      </c>
+        <v>-9.5</v>
+      </c>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -987,7 +975,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7.6</v>
+        <v>7.9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -1001,7 +989,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Louisville -6.6</t>
+          <t>Louisville -6.9</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -1031,41 +1019,41 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Texas Tech</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7.1</v>
+        <v>7.4</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Ohio State -nan</t>
+          <t>Arkansas -2.5</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Ohio State -7.5</t>
+          <t>Texas Tech -3.5</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Ohio State -14.6</t>
+          <t>Arkansas -3.9</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>7.5</v>
+        <v>-3.5</v>
       </c>
       <c r="I12" t="n">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Ohio State -25.0</t>
+          <t>Arkansas -13.0</t>
         </is>
       </c>
       <c r="K12" t="n">
@@ -1084,51 +1072,51 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Fresno State</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Northern Illinois</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>6.4</v>
+        <v>6.1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Notre Dame -nan</t>
+          <t>Fresno State -nan</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Notre Dame -7</t>
+          <t>Northern Illinois -2</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Notre Dame -13.4</t>
+          <t>Fresno State -4.1</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>7</v>
+        <v>-2</v>
       </c>
       <c r="I13" t="n">
-        <v>10</v>
+        <v>-8</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Notre Dame -10.0</t>
+          <t>Northern Illinois -8.0</t>
         </is>
       </c>
       <c r="K13" t="n">
         <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1137,51 +1125,51 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fresno State</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Northern Illinois</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Fresno State -nan</t>
+          <t>Ohio State -nan</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Northern Illinois -2</t>
+          <t>Ohio State -7.5</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Fresno State -3.8</t>
+          <t>Ohio State -13.5</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>-2</v>
+        <v>7.5</v>
       </c>
       <c r="I14" t="n">
-        <v>-8</v>
+        <v>25</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Northern Illinois -8.0</t>
+          <t>Ohio State -25.0</t>
         </is>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1190,41 +1178,41 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>Texas State</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>North Texas</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.8</v>
+        <v>5.5</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Colorado State -nan</t>
+          <t>Texas State -nan</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Miami (OH) -1</t>
+          <t>Texas State -15.5</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Miami (OH) -6.8</t>
+          <t>Texas State -10.0</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>-1</v>
+        <v>15.5</v>
       </c>
       <c r="I15" t="n">
-        <v>-26</v>
+        <v>2</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Miami (OH) -26.0</t>
+          <t>Texas State -2.0</t>
         </is>
       </c>
       <c r="K15" t="n">
@@ -1243,41 +1231,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5.8</v>
+        <v>5.5</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Georgia -nan</t>
+          <t>Colorado State -nan</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Notre Dame -1</t>
+          <t>Miami (OH) -1</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Notre Dame -6.8</t>
+          <t>Miami (OH) -6.5</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>-1</v>
       </c>
       <c r="I16" t="n">
-        <v>-13</v>
+        <v>-26</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Notre Dame -13.0</t>
+          <t>Miami (OH) -26.0</t>
         </is>
       </c>
       <c r="K16" t="n">
@@ -1296,41 +1284,41 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Texas State</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>North Texas</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.699999999999999</v>
+        <v>5.199999999999999</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Texas State -nan</t>
+          <t>Michigan -nan</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Texas State -15.5</t>
+          <t>Alabama -16.5</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Texas State -9.8</t>
+          <t>Alabama -11.3</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>15.5</v>
+        <v>-16.5</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Texas State -2.0</t>
+          <t>Michigan -6.0</t>
         </is>
       </c>
       <c r="K17" t="n">
@@ -1340,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1349,51 +1337,51 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>5.300000000000001</v>
+        <v>5.1</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Michigan -nan</t>
+          <t>Florida -nan</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Alabama -16.5</t>
+          <t>Florida -10</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Alabama -11.2</t>
+          <t>Florida -4.9</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>-16.5</v>
+        <v>10</v>
       </c>
       <c r="I18" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Michigan -6.0</t>
+          <t>Florida -25.0</t>
         </is>
       </c>
       <c r="K18" t="n">
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1411,7 +1399,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>5.1</v>
+        <v>4.8</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -1425,7 +1413,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Ohio -1.4</t>
+          <t>Ohio -1.7</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1451,52 +1439,52 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.9</v>
+        <v>4.300000000000001</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Florida -nan</t>
+          <t>Memphis -2.0</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Florida -10</t>
+          <t>Memphis -5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Florida -5.1</t>
+          <t>Memphis -9.3</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="I20" t="n">
-        <v>25</v>
+        <v>-5</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Florida -25.0</t>
+          <t>Memphis -5.0</t>
         </is>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
         <v>1</v>
@@ -1504,7 +1492,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1517,7 +1505,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4.3</v>
+        <v>4.2</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1531,7 +1519,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>North Carolina -6.3</t>
+          <t>North Carolina -6.2</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1557,45 +1545,45 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>4.1</v>
+        <v>4.2</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>San José State -2.5</t>
+          <t>Georgia -nan</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>South Florida -1.5</t>
+          <t>Notre Dame -1</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>South Florida -5.6</t>
+          <t>Notre Dame -5.2</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>-1.5</v>
+        <v>-1</v>
       </c>
       <c r="I22" t="n">
-        <v>-2</v>
+        <v>-13</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>South Florida -2.0</t>
+          <t>Notre Dame -13.0</t>
         </is>
       </c>
       <c r="K22" t="n">
@@ -1610,16 +1598,16 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1627,28 +1615,28 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Ohio State -2.5</t>
+          <t>San José State -2.5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Ohio State -2.5</t>
+          <t>South Florida -1.5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Ohio State -6.5</t>
+          <t>South Florida -5.5</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>-2.5</v>
+        <v>-1.5</v>
       </c>
       <c r="I23" t="n">
-        <v>-20</v>
+        <v>-2</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Ohio State -20.0</t>
+          <t>South Florida -2.0</t>
         </is>
       </c>
       <c r="K23" t="n">
@@ -1663,105 +1651,105 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Memphis -2.0</t>
+          <t>Iowa State -1.0</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Memphis -5</t>
+          <t>Miami -5</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Memphis -9.0</t>
+          <t>Miami -8.9</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>-5</v>
+        <v>5</v>
       </c>
       <c r="I24" t="n">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Memphis -5.0</t>
+          <t>Iowa State -1.0</t>
         </is>
       </c>
       <c r="K24" t="n">
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.800000000000001</v>
+        <v>3.4</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Iowa State -1.0</t>
+          <t>NC State -nan</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Miami -5</t>
+          <t>NC State -7.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Miami -8.8</t>
+          <t>NC State -4.1</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>5</v>
+        <v>7.5</v>
       </c>
       <c r="I25" t="n">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Iowa State -1.0</t>
+          <t>East Carolina -5.0</t>
         </is>
       </c>
       <c r="K25" t="n">
         <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25" t="n">
         <v>0</v>
@@ -1769,45 +1757,45 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3</v>
+        <v>3.1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>NC State -nan</t>
+          <t>Vanderbilt -nan</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>NC State -7.5</t>
+          <t>Georgia Tech -3</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>NC State -4.5</t>
+          <t>Vanderbilt -0.1</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>7.5</v>
+        <v>-3</v>
       </c>
       <c r="I26" t="n">
-        <v>-5</v>
+        <v>8</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>East Carolina -5.0</t>
+          <t>Vanderbilt -8.0</t>
         </is>
       </c>
       <c r="K26" t="n">
@@ -1817,50 +1805,50 @@
         <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sam Houston</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Georgia Southern</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2.9</v>
+        <v>3</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Sam Houston -nan</t>
+          <t>Ohio State -2.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Georgia Southern -3.5</t>
+          <t>Ohio State -2.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Georgia Southern -0.6</t>
+          <t>Ohio State -5.5</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>-3.5</v>
+        <v>-2.5</v>
       </c>
       <c r="I27" t="n">
-        <v>5</v>
+        <v>-20</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Sam Houston -5.0</t>
+          <t>Ohio State -20.0</t>
         </is>
       </c>
       <c r="K27" t="n">
@@ -1870,57 +1858,57 @@
         <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Toledo</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Pittsburgh</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.7</v>
+        <v>2.800000000000001</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Vanderbilt -nan</t>
+          <t>Pittsburgh -9.5</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Georgia Tech -3</t>
+          <t>Pittsburgh -6.5</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Georgia Tech -0.3</t>
+          <t>Pittsburgh -9.3</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>-3</v>
+        <v>-6.5</v>
       </c>
       <c r="I28" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Vanderbilt -8.0</t>
+          <t>Toledo -2.0</t>
         </is>
       </c>
       <c r="K28" t="n">
         <v>1</v>
       </c>
       <c r="L28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M28" t="n">
         <v>0</v>
@@ -1928,52 +1916,52 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Toledo</t>
+          <t>Sam Houston</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Pittsburgh</t>
+          <t>Georgia Southern</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2.699999999999999</v>
+        <v>2.6</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Pittsburgh -9.5</t>
+          <t>Sam Houston -nan</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Pittsburgh -6.5</t>
+          <t>Georgia Southern -3.5</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pittsburgh -9.2</t>
+          <t>Georgia Southern -0.9</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>-6.5</v>
+        <v>-3.5</v>
       </c>
       <c r="I29" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Toledo -2.0</t>
+          <t>Sam Houston -5.0</t>
         </is>
       </c>
       <c r="K29" t="n">
         <v>1</v>
       </c>
       <c r="L29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M29" t="n">
         <v>0</v>
@@ -1981,52 +1969,52 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2.6</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Boise State -nan</t>
+          <t>UTSA -nan</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Penn State -12</t>
+          <t>UTSA -12.5</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Penn State -14.6</t>
+          <t>UTSA -10.2</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>-12</v>
+        <v>12.5</v>
       </c>
       <c r="I30" t="n">
-        <v>-17</v>
+        <v>29</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Penn State -17.0</t>
+          <t>UTSA -29.0</t>
         </is>
       </c>
       <c r="K30" t="n">
         <v>1</v>
       </c>
       <c r="L30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M30" t="n">
         <v>1</v>
@@ -2034,45 +2022,45 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.4</v>
+        <v>2.3</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>UTSA -nan</t>
+          <t>Missouri -nan</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>UTSA -12.5</t>
+          <t>Missouri -1</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>UTSA -10.1</t>
+          <t>Iowa -1.3</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>12.5</v>
+        <v>1</v>
       </c>
       <c r="I31" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>UTSA -29.0</t>
+          <t>Missouri -3.0</t>
         </is>
       </c>
       <c r="K31" t="n">
@@ -2082,103 +2070,103 @@
         <v>0</v>
       </c>
       <c r="M31" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Missouri -nan</t>
+          <t>TCU -nan</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Missouri -1</t>
+          <t>TCU -9.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Iowa -1.4</t>
+          <t>TCU -11.5</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>1</v>
+        <v>9.5</v>
       </c>
       <c r="I32" t="n">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Missouri -3.0</t>
+          <t>TCU -31.0</t>
         </is>
       </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>Arizona State</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1.800000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>TCU -nan</t>
+          <t>Arizona State -nan</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>TCU -9.5</t>
+          <t>Texas -13.5</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>TCU -11.3</t>
+          <t>Texas -11.6</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>9.5</v>
+        <v>-13.5</v>
       </c>
       <c r="I33" t="n">
-        <v>31</v>
+        <v>-8</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>TCU -31.0</t>
+          <t>Texas -8.0</t>
         </is>
       </c>
       <c r="K33" t="n">
@@ -2193,7 +2181,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2246,45 +2234,45 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.600000000000001</v>
+        <v>1.5</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Army -nan</t>
+          <t>Illinois -nan</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Army -15</t>
+          <t>South Carolina -9.5</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Army -16.6</t>
+          <t>South Carolina -8.0</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>15</v>
+        <v>-9.5</v>
       </c>
       <c r="I35" t="n">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Army -21.0</t>
+          <t>Illinois -4.0</t>
         </is>
       </c>
       <c r="K35" t="n">
@@ -2294,50 +2282,50 @@
         <v>1</v>
       </c>
       <c r="M35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Nebraska -nan</t>
+          <t>Boise State -nan</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Nebraska -3</t>
+          <t>Penn State -12</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Nebraska -4.5</t>
+          <t>Penn State -13.4</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>3</v>
+        <v>-12</v>
       </c>
       <c r="I36" t="n">
-        <v>5</v>
+        <v>-17</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Nebraska -5.0</t>
+          <t>Penn State -17.0</t>
         </is>
       </c>
       <c r="K36" t="n">
@@ -2352,45 +2340,45 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.5</v>
+        <v>1.300000000000001</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Illinois -nan</t>
+          <t>Army -nan</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>South Carolina -9.5</t>
+          <t>Army -15</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>South Carolina -8.0</t>
+          <t>Army -16.3</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>-9.5</v>
+        <v>15</v>
       </c>
       <c r="I37" t="n">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Illinois -4.0</t>
+          <t>Army -21.0</t>
         </is>
       </c>
       <c r="K37" t="n">
@@ -2400,21 +2388,21 @@
         <v>1</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>UNLV</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>California</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -2422,35 +2410,35 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>UNLV -nan</t>
+          <t>Nebraska -nan</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>UNLV -3</t>
+          <t>Nebraska -3</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>UNLV -1.7</t>
+          <t>Nebraska -4.3</t>
         </is>
       </c>
       <c r="H38" t="n">
         <v>3</v>
       </c>
       <c r="I38" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>UNLV -11.0</t>
+          <t>Nebraska -5.0</t>
         </is>
       </c>
       <c r="K38" t="n">
         <v>1</v>
       </c>
       <c r="L38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M38" t="n">
         <v>1</v>
@@ -2458,98 +2446,98 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>UNLV</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>California</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.2</v>
+        <v>1.1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>USC -nan</t>
+          <t>UNLV -nan</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -3.5</t>
+          <t>UNLV -3</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.3</t>
+          <t>UNLV -1.9</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>-3.5</v>
+        <v>3</v>
       </c>
       <c r="I39" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>USC -4.0</t>
+          <t>UNLV -11.0</t>
         </is>
       </c>
       <c r="K39" t="n">
         <v>1</v>
       </c>
       <c r="L39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M39" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>James Madison -nan</t>
+          <t>USC -nan</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>James Madison -7.5</t>
+          <t>Texas A&amp;M -3.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>James Madison -8.5</t>
+          <t>Texas A&amp;M -2.6</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>7.5</v>
+        <v>-3.5</v>
       </c>
       <c r="I40" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>James Madison -10.0</t>
+          <t>USC -4.0</t>
         </is>
       </c>
       <c r="K40" t="n">
@@ -2559,50 +2547,50 @@
         <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>1</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Texas -nan</t>
+          <t>James Madison -nan</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Texas -13.5</t>
+          <t>James Madison -7.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Texas -14.5</t>
+          <t>James Madison -8.3</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>13.5</v>
+        <v>7.5</v>
       </c>
       <c r="I41" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Texas -14.0</t>
+          <t>James Madison -10.0</t>
         </is>
       </c>
       <c r="K41" t="n">
@@ -2617,24 +2605,24 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Arizona State</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Clemson</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.5</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Arizona State -nan</t>
+          <t>Texas -nan</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2644,25 +2632,25 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Texas -13.0</t>
+          <t>Texas -13.1</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>-13.5</v>
+        <v>13.5</v>
       </c>
       <c r="I42" t="n">
-        <v>-8</v>
+        <v>14</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Texas -8.0</t>
+          <t>Texas -14.0</t>
         </is>
       </c>
       <c r="K42" t="n">
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M42" t="n">
         <v>1</v>
@@ -2670,7 +2658,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -2683,7 +2671,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.2000000000000002</v>
+        <v>0.4000000000000004</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2697,7 +2685,7 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Kansas State -7.3</t>
+          <t>Kansas State -7.1</t>
         </is>
       </c>
       <c r="H43" t="n">
@@ -2723,7 +2711,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2736,7 +2724,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.1999999999999993</v>
+        <v>0</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -2750,7 +2738,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Bowling Green -10.7</t>
+          <t>Bowling Green -10.5</t>
         </is>
       </c>
       <c r="H44" t="n">
@@ -2768,7 +2756,7 @@
         <v>0</v>
       </c>
       <c r="L44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M44" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
updating everything with updating power ratings
</commit_message>
<xml_diff>
--- a/ESCAPE Ratings/Spreads/y2024/spreads_tracker_week17.xlsx
+++ b/ESCAPE Ratings/Spreads/y2024/spreads_tracker_week17.xlsx
@@ -535,7 +535,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Buffalo -19.0</t>
+          <t>Buffalo -19</t>
         </is>
       </c>
       <c r="K2" t="n">
@@ -588,7 +588,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>LSU -13.0</t>
+          <t>LSU -13</t>
         </is>
       </c>
       <c r="K3" t="n">
@@ -641,7 +641,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Syracuse -17.0</t>
+          <t>Syracuse -17</t>
         </is>
       </c>
       <c r="K4" t="n">
@@ -669,7 +669,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>10</v>
+        <v>9.9</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -683,7 +683,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Minnesota -0.0</t>
+          <t>Minnesota -0.1</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -694,7 +694,7 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Minnesota -14.0</t>
+          <t>Minnesota -14</t>
         </is>
       </c>
       <c r="K5" t="n">
@@ -704,7 +704,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -747,7 +747,7 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Navy -1.0</t>
+          <t>Navy -1</t>
         </is>
       </c>
       <c r="K6" t="n">
@@ -775,7 +775,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>8.5</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -789,7 +789,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Penn State -17.5</t>
+          <t>Penn State -17.2</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -800,7 +800,7 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Penn State -28.0</t>
+          <t>Penn State -28</t>
         </is>
       </c>
       <c r="K7" t="n">
@@ -819,45 +819,45 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Western Michigan</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>South Alabama</t>
+          <t>Louisville</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>8</v>
+        <v>7.9</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>South Alabama -10.0</t>
+          <t>Washington -nan</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>South Alabama -6</t>
+          <t>Washington -1</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>South Alabama -14.0</t>
+          <t>Louisville -6.9</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>-6</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>-7</v>
+        <v>-1</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>South Alabama -7.0</t>
+          <t>Louisville -1</t>
         </is>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -872,51 +872,51 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Western Michigan</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>BYU</t>
+          <t>South Alabama</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>7.9</v>
+        <v>7.5</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Colorado -nan</t>
+          <t>South Alabama -10.0</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Colorado -3</t>
+          <t>South Alabama -6</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Colorado -10.9</t>
+          <t>South Alabama -13.5</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>3</v>
+        <v>-6</v>
       </c>
       <c r="I9" t="n">
-        <v>-22</v>
+        <v>-7</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>BYU -22.0</t>
+          <t>South Alabama -7</t>
         </is>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -925,40 +925,52 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7.9</v>
+        <v>7.300000000000001</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Notre Dame -nan</t>
+          <t>Ohio State -nan</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Ohio State -9.5</t>
+          <t>Ohio State -7.5</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Ohio State -1.6</t>
+          <t>Ohio State -14.8</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>-9.5</v>
-      </c>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
+        <v>7.5</v>
+      </c>
+      <c r="I10" t="n">
+        <v>25</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Ohio State -25</t>
+        </is>
+      </c>
+      <c r="K10" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -966,51 +978,51 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Colorado</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Louisville</t>
+          <t>BYU</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7.9</v>
+        <v>6.9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Washington -nan</t>
+          <t>Colorado -nan</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Washington -1</t>
+          <t>Colorado -3</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Louisville -6.9</t>
+          <t>Colorado -9.9</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I11" t="n">
-        <v>-1</v>
+        <v>-22</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Louisville -1.0</t>
+          <t>BYU -22</t>
         </is>
       </c>
       <c r="K11" t="n">
         <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1028,7 +1040,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>7.4</v>
+        <v>6.8</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1042,7 +1054,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Arkansas -3.9</t>
+          <t>Arkansas -3.3</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -1053,7 +1065,7 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Arkansas -13.0</t>
+          <t>Arkansas -13</t>
         </is>
       </c>
       <c r="K12" t="n">
@@ -1106,7 +1118,7 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Northern Illinois -8.0</t>
+          <t>Northern Illinois -8</t>
         </is>
       </c>
       <c r="K13" t="n">
@@ -1125,48 +1137,48 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Tennessee</t>
+          <t>Tulane</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>5.4</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Ohio State -nan</t>
+          <t>Florida -nan</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Ohio State -7.5</t>
+          <t>Florida -10</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Ohio State -13.5</t>
+          <t>Florida -4.6</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>7.5</v>
+        <v>10</v>
       </c>
       <c r="I14" t="n">
         <v>25</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Ohio State -25.0</t>
+          <t>Florida -25</t>
         </is>
       </c>
       <c r="K14" t="n">
         <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M14" t="n">
         <v>1</v>
@@ -1187,7 +1199,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.5</v>
+        <v>5.300000000000001</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -1201,7 +1213,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Texas State -10.0</t>
+          <t>Texas State -10.2</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1212,7 +1224,7 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Texas State -2.0</t>
+          <t>Texas State -2</t>
         </is>
       </c>
       <c r="K15" t="n">
@@ -1231,41 +1243,41 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Colorado State</t>
+          <t>West Virginia</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Miami (OH)</t>
+          <t>Memphis</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>5.5</v>
+        <v>4.9</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Colorado State -nan</t>
+          <t>Memphis -2.0</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Miami (OH) -1</t>
+          <t>Memphis -5</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Miami (OH) -6.5</t>
+          <t>Memphis -9.9</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="I16" t="n">
-        <v>-26</v>
+        <v>-5</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Miami (OH) -26.0</t>
+          <t>Memphis -5</t>
         </is>
       </c>
       <c r="K16" t="n">
@@ -1293,7 +1305,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>5.199999999999999</v>
+        <v>4.699999999999999</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -1307,7 +1319,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Alabama -11.3</t>
+          <t>Alabama -11.8</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1318,7 +1330,7 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Michigan -6.0</t>
+          <t>Michigan -6</t>
         </is>
       </c>
       <c r="K17" t="n">
@@ -1337,48 +1349,48 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Vanderbilt</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Tulane</t>
+          <t>Georgia Tech</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>5.1</v>
+        <v>4.5</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Florida -nan</t>
+          <t>Vanderbilt -nan</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Florida -10</t>
+          <t>Georgia Tech -3</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Florida -4.9</t>
+          <t>Vanderbilt -1.5</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>10</v>
+        <v>-3</v>
       </c>
       <c r="I18" t="n">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Florida -25.0</t>
+          <t>Vanderbilt -8</t>
         </is>
       </c>
       <c r="K18" t="n">
         <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18" t="n">
         <v>1</v>
@@ -1390,45 +1402,45 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Jacksonville State</t>
+          <t>Colorado State</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Ohio</t>
+          <t>Miami (OH)</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4.8</v>
+        <v>4.4</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Ohio -2.5</t>
+          <t>Colorado State -nan</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Ohio -6.5</t>
+          <t>Miami (OH) -1</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Ohio -1.7</t>
+          <t>Miami (OH) -5.4</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>-6.5</v>
+        <v>-1</v>
       </c>
       <c r="I19" t="n">
-        <v>-3</v>
+        <v>-26</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Ohio -3.0</t>
+          <t>Miami (OH) -26</t>
         </is>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" t="n">
         <v>1</v>
@@ -1439,52 +1451,52 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>West Virginia</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Memphis</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>4.300000000000001</v>
+        <v>4.3</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Memphis -2.0</t>
+          <t>Notre Dame -nan</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Memphis -5</t>
+          <t>Ohio State -8.5</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Memphis -9.3</t>
+          <t>Ohio State -4.2</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>-5</v>
+        <v>-8.5</v>
       </c>
       <c r="I20" t="n">
-        <v>-5</v>
+        <v>-11</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Memphis -5.0</t>
+          <t>Ohio State -11</t>
         </is>
       </c>
       <c r="K20" t="n">
         <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M20" t="n">
         <v>1</v>
@@ -1492,7 +1504,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1530,7 +1542,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>UConn -13.0</t>
+          <t>UConn -13</t>
         </is>
       </c>
       <c r="K21" t="n">
@@ -1545,16 +1557,16 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>NC State</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Notre Dame</t>
+          <t>East Carolina</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -1562,28 +1574,28 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Georgia -nan</t>
+          <t>NC State -nan</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Notre Dame -1</t>
+          <t>NC State -7.5</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Notre Dame -5.2</t>
+          <t>NC State -3.3</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>-1</v>
+        <v>7.5</v>
       </c>
       <c r="I22" t="n">
-        <v>-13</v>
+        <v>-5</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Notre Dame -13.0</t>
+          <t>East Carolina -5</t>
         </is>
       </c>
       <c r="K22" t="n">
@@ -1593,74 +1605,74 @@
         <v>1</v>
       </c>
       <c r="M22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>San José State</t>
+          <t>Miami</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>South Florida</t>
+          <t>Iowa State</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>4</v>
+        <v>3.9</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>San José State -2.5</t>
+          <t>Iowa State -1.0</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>South Florida -1.5</t>
+          <t>Miami -5</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>South Florida -5.5</t>
+          <t>Miami -8.9</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>-1.5</v>
+        <v>5</v>
       </c>
       <c r="I23" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>South Florida -2.0</t>
+          <t>Iowa State -1</t>
         </is>
       </c>
       <c r="K23" t="n">
         <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Miami</t>
+          <t>Georgia</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Iowa State</t>
+          <t>Notre Dame</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -1668,81 +1680,81 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Iowa State -1.0</t>
+          <t>Georgia -nan</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Miami -5</t>
+          <t>Notre Dame -1</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Miami -8.9</t>
+          <t>Notre Dame -4.9</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="I24" t="n">
-        <v>-1</v>
+        <v>-13</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Iowa State -1.0</t>
+          <t>Notre Dame -13</t>
         </is>
       </c>
       <c r="K24" t="n">
         <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NC State</t>
+          <t>Jacksonville State</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>East Carolina</t>
+          <t>Ohio</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.4</v>
+        <v>3.8</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>NC State -nan</t>
+          <t>Ohio -2.5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>NC State -7.5</t>
+          <t>Ohio -6.5</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>NC State -4.1</t>
+          <t>Ohio -2.7</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>7.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I25" t="n">
-        <v>-5</v>
+        <v>-3</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>East Carolina -5.0</t>
+          <t>Ohio -3</t>
         </is>
       </c>
       <c r="K25" t="n">
@@ -1752,50 +1764,50 @@
         <v>1</v>
       </c>
       <c r="M25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Vanderbilt</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Georgia Tech</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>3.1</v>
+        <v>3.8</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Vanderbilt -nan</t>
+          <t>Ohio State -2.5</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Georgia Tech -3</t>
+          <t>Ohio State -2.5</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Vanderbilt -0.1</t>
+          <t>Ohio State -6.3</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>-3</v>
+        <v>-2.5</v>
       </c>
       <c r="I26" t="n">
-        <v>8</v>
+        <v>-20</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Vanderbilt -8.0</t>
+          <t>Ohio State -20</t>
         </is>
       </c>
       <c r="K26" t="n">
@@ -1810,45 +1822,45 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Oregon</t>
+          <t>San José State</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Ohio State</t>
+          <t>South Florida</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>3</v>
+        <v>3.7</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Ohio State -2.5</t>
+          <t>San José State -2.5</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Ohio State -2.5</t>
+          <t>South Florida -1.5</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Ohio State -5.5</t>
+          <t>South Florida -5.2</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>-2.5</v>
+        <v>-1.5</v>
       </c>
       <c r="I27" t="n">
-        <v>-20</v>
+        <v>-2</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Ohio State -20.0</t>
+          <t>South Florida -2</t>
         </is>
       </c>
       <c r="K27" t="n">
@@ -1863,7 +1875,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1876,7 +1888,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2.800000000000001</v>
+        <v>3.1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1890,7 +1902,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Pittsburgh -9.3</t>
+          <t>Pittsburgh -9.6</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1901,11 +1913,11 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Toledo -2.0</t>
+          <t>Toledo -2</t>
         </is>
       </c>
       <c r="K28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" t="n">
         <v>0</v>
@@ -1916,7 +1928,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1929,7 +1941,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>2.6</v>
+        <v>2.8</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1943,7 +1955,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Georgia Southern -0.9</t>
+          <t>Georgia Southern -0.7</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1954,7 +1966,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Sam Houston -5.0</t>
+          <t>Sam Houston -5</t>
         </is>
       </c>
       <c r="K29" t="n">
@@ -1973,41 +1985,41 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>UTSA</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Coastal Carolina</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>2.300000000000001</v>
+        <v>2.4</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>UTSA -nan</t>
+          <t>Missouri -nan</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>UTSA -12.5</t>
+          <t>Missouri -1</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>UTSA -10.2</t>
+          <t>Iowa -1.4</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>12.5</v>
+        <v>1</v>
       </c>
       <c r="I30" t="n">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>UTSA -29.0</t>
+          <t>Missouri -3</t>
         </is>
       </c>
       <c r="K30" t="n">
@@ -2017,7 +2029,7 @@
         <v>0</v>
       </c>
       <c r="M30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -2026,48 +2038,48 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>South Carolina</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>2.3</v>
+        <v>2.2</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Missouri -nan</t>
+          <t>Illinois -nan</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Missouri -1</t>
+          <t>South Carolina -9.5</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Iowa -1.3</t>
+          <t>South Carolina -7.3</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>1</v>
+        <v>-9.5</v>
       </c>
       <c r="I31" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Missouri -3.0</t>
+          <t>Illinois -4</t>
         </is>
       </c>
       <c r="K31" t="n">
         <v>1</v>
       </c>
       <c r="L31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" t="n">
         <v>0</v>
@@ -2079,12 +2091,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>TCU</t>
+          <t>UTSA</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Coastal Carolina</t>
         </is>
       </c>
       <c r="D32" t="n">
@@ -2092,35 +2104,35 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>TCU -nan</t>
+          <t>UTSA -nan</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>TCU -9.5</t>
+          <t>UTSA -12.5</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>TCU -11.5</t>
+          <t>UTSA -10.5</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>9.5</v>
+        <v>12.5</v>
       </c>
       <c r="I32" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>TCU -31.0</t>
+          <t>UTSA -29</t>
         </is>
       </c>
       <c r="K32" t="n">
         <v>1</v>
       </c>
       <c r="L32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M32" t="n">
         <v>1</v>
@@ -2166,7 +2178,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Texas -8.0</t>
+          <t>Texas -8</t>
         </is>
       </c>
       <c r="K33" t="n">
@@ -2185,41 +2197,41 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ole Miss</t>
+          <t>Army</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Duke</t>
+          <t>Louisiana Tech</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>1.699999999999999</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Ole Miss -nan</t>
+          <t>Army -nan</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Ole Miss -17.5</t>
+          <t>Army -15</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Ole Miss -19.2</t>
+          <t>Army -16.8</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>17.5</v>
+        <v>15</v>
       </c>
       <c r="I34" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Ole Miss -32.0</t>
+          <t>Army -21</t>
         </is>
       </c>
       <c r="K34" t="n">
@@ -2238,41 +2250,41 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>South Carolina</t>
+          <t>Boston College</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Illinois -nan</t>
+          <t>Nebraska -nan</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>South Carolina -9.5</t>
+          <t>Nebraska -3</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>South Carolina -8.0</t>
+          <t>Nebraska -4.3</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>-9.5</v>
+        <v>3</v>
       </c>
       <c r="I35" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Illinois -4.0</t>
+          <t>Nebraska -5</t>
         </is>
       </c>
       <c r="K35" t="n">
@@ -2282,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="M35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
@@ -2291,41 +2303,41 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Boise State</t>
+          <t>USC</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Penn State</t>
+          <t>Texas A&amp;M</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Boise State -nan</t>
+          <t>USC -nan</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Penn State -12</t>
+          <t>Texas A&amp;M -3.5</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Penn State -13.4</t>
+          <t>Texas A&amp;M -2.2</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>-12</v>
+        <v>-3.5</v>
       </c>
       <c r="I36" t="n">
-        <v>-17</v>
+        <v>4</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Penn State -17.0</t>
+          <t>USC -4</t>
         </is>
       </c>
       <c r="K36" t="n">
@@ -2335,7 +2347,7 @@
         <v>1</v>
       </c>
       <c r="M36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2344,41 +2356,41 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Army</t>
+          <t>TCU</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Louisiana Tech</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>1.300000000000001</v>
+        <v>1.199999999999999</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Army -nan</t>
+          <t>TCU -nan</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Army -15</t>
+          <t>TCU -9.5</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Army -16.3</t>
+          <t>TCU -10.7</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>15</v>
+        <v>9.5</v>
       </c>
       <c r="I37" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Army -21.0</t>
+          <t>TCU -31</t>
         </is>
       </c>
       <c r="K37" t="n">
@@ -2397,51 +2409,51 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Bowling Green</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Boston College</t>
+          <t>Arkansas State</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>1.3</v>
+        <v>1.1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Nebraska -nan</t>
+          <t>Bowling Green -6.5</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Nebraska -3</t>
+          <t>Bowling Green -10.5</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Nebraska -4.3</t>
+          <t>Bowling Green -9.4</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>3</v>
+        <v>10.5</v>
       </c>
       <c r="I38" t="n">
-        <v>5</v>
+        <v>-7</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Nebraska -5.0</t>
+          <t>Arkansas State -7</t>
         </is>
       </c>
       <c r="K38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L38" t="n">
         <v>1</v>
       </c>
       <c r="M38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2459,7 +2471,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>1.1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2473,7 +2485,7 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>UNLV -1.9</t>
+          <t>UNLV -2.1</t>
         </is>
       </c>
       <c r="H39" t="n">
@@ -2484,7 +2496,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>UNLV -11.0</t>
+          <t>UNLV -11</t>
         </is>
       </c>
       <c r="K39" t="n">
@@ -2503,41 +2515,41 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>USC</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Texas A&amp;M</t>
+          <t>Ohio State</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>0.8999999999999999</v>
+        <v>0.7999999999999998</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>USC -nan</t>
+          <t>Texas -nan</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -3.5</t>
+          <t>Ohio State -6.5</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Texas A&amp;M -2.6</t>
+          <t>Ohio State -7.3</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>-3.5</v>
+        <v>-6.5</v>
       </c>
       <c r="I40" t="n">
-        <v>4</v>
+        <v>-14</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>USC -4.0</t>
+          <t>Ohio State -14</t>
         </is>
       </c>
       <c r="K40" t="n">
@@ -2547,7 +2559,7 @@
         <v>1</v>
       </c>
       <c r="M40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
@@ -2556,41 +2568,41 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>James Madison</t>
+          <t>Ole Miss</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Western Kentucky</t>
+          <t>Duke</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.8000000000000007</v>
+        <v>0.6999999999999993</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>James Madison -nan</t>
+          <t>Ole Miss -nan</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>James Madison -7.5</t>
+          <t>Ole Miss -17.5</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>James Madison -8.3</t>
+          <t>Ole Miss -18.2</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>7.5</v>
+        <v>17.5</v>
       </c>
       <c r="I41" t="n">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>James Madison -10.0</t>
+          <t>Ole Miss -32</t>
         </is>
       </c>
       <c r="K41" t="n">
@@ -2609,48 +2621,48 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Kansas State</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Clemson</t>
+          <t>Rutgers</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5999999999999996</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Texas -nan</t>
+          <t>Kansas State -7.0</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Texas -13.5</t>
+          <t>Kansas State -7.5</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Texas -13.1</t>
+          <t>Kansas State -6.9</t>
         </is>
       </c>
       <c r="H42" t="n">
-        <v>13.5</v>
+        <v>7.5</v>
       </c>
       <c r="I42" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Texas -14.0</t>
+          <t>Kansas State -3</t>
         </is>
       </c>
       <c r="K42" t="n">
         <v>1</v>
       </c>
       <c r="L42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M42" t="n">
         <v>1</v>
@@ -2662,45 +2674,45 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Kansas State</t>
+          <t>James Madison</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Rutgers</t>
+          <t>Western Kentucky</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>0.4000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Kansas State -7.0</t>
+          <t>James Madison -nan</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Kansas State -7.5</t>
+          <t>James Madison -7.5</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Kansas State -7.1</t>
+          <t>James Madison -8.0</t>
         </is>
       </c>
       <c r="H43" t="n">
         <v>7.5</v>
       </c>
       <c r="I43" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Kansas State -3.0</t>
+          <t>James Madison -10</t>
         </is>
       </c>
       <c r="K43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L43" t="n">
         <v>1</v>
@@ -2715,51 +2727,51 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Bowling Green</t>
+          <t>Boise State</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arkansas State</t>
+          <t>Penn State</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0</v>
+        <v>0.09999999999999964</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Bowling Green -6.5</t>
+          <t>Boise State -nan</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Bowling Green -10.5</t>
+          <t>Penn State -12</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Bowling Green -10.5</t>
+          <t>Penn State -11.9</t>
         </is>
       </c>
       <c r="H44" t="n">
-        <v>10.5</v>
+        <v>-12</v>
       </c>
       <c r="I44" t="n">
-        <v>-7</v>
+        <v>-17</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Arkansas State -7.0</t>
+          <t>Penn State -17</t>
         </is>
       </c>
       <c r="K44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>